<commit_message>
added b-h testing script and also replot script for pred50
</commit_message>
<xml_diff>
--- a/data/UseCaseWeighting/7-9/data_points_accuracy_7_11.xlsx
+++ b/data/UseCaseWeighting/7-9/data_points_accuracy_7_11.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17460" windowHeight="8808" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17460" windowHeight="8805" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="False Discovery Rate" sheetId="2" r:id="rId1"/>
@@ -1104,9 +1104,9 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1120,27 +1120,27 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1154,27 +1154,27 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1188,27 +1188,27 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1222,22 +1222,22 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1255,23 +1255,23 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" customWidth="1"/>
-    <col min="20" max="20" width="18.6640625" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="20" max="20" width="18.7109375" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" customWidth="1"/>
     <col min="26" max="26" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>7.5000000740740966E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>0.883476598</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>0.268117713813674</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1851,17 +1851,17 @@
       </c>
       <c r="P13" s="2"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>58</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E18">
         <f>(E4-E2)/SQRT(F4^2/10+F2^2/10)</f>
         <v>2.0897288898007096</v>
@@ -1895,7 +1895,7 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E19">
         <f>(E8-E6)/SQRT(F8^2/10+F6^2/10)</f>
         <v>7.0207075885885919</v>
@@ -1909,7 +1909,7 @@
         <v>17.938296685533214</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E20">
         <f>(E12-E10)/SQRT(F10^2/10+F12^2/10)</f>
         <v>2.5077139058619347</v>
@@ -1923,17 +1923,17 @@
         <v>9.2833765053183352</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>58</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>12</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>3.0297345913140425</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>11</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>3.6129552463040615</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>60</v>
       </c>
@@ -1996,34 +1996,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="X74" sqref="X74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.77734375" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" customWidth="1"/>
-    <col min="10" max="10" width="19.109375" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" customWidth="1"/>
-    <col min="14" max="14" width="18.44140625" customWidth="1"/>
-    <col min="15" max="15" width="20.77734375" customWidth="1"/>
-    <col min="16" max="16" width="23.88671875" customWidth="1"/>
-    <col min="17" max="17" width="20.33203125" customWidth="1"/>
-    <col min="20" max="20" width="18.6640625" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="23.85546875" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" customWidth="1"/>
+    <col min="20" max="20" width="18.7109375" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" customWidth="1"/>
     <col min="26" max="26" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>7.5000000740740966E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>8.611111397849483E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>6.8098064139197348E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>8.611111397849483E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>2.1821782477062523E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>4.6569533515100771E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>4.6569533515100771E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>4.4896104995469761E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>5.425935235089957E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>3.8173395732912029E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>3.8972096679025112E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>5.7455169198194433E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0.27706659</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>0.73431679999999999</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>0.66666669999999995</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>5.3700350000000001E-2</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>1.01997396</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>1.8482500399999999</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>0.3333333</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>0.82374561999999996</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>0.3333333</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>0.27362692</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>3.9690900000000001E-2</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>1.5832008500000001</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>0.66666669999999995</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>0.49117488999999998</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>63</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>0.47499999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -3208,76 +3208,76 @@
         <v>0.27230725202640726</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
       <c r="B28">
-        <f>STDEV(B16:B25)/SQRT(10)</f>
+        <f t="shared" ref="B28:Q28" si="16">STDEV(B16:B25)/SQRT(10)</f>
         <v>0.19644865400312733</v>
       </c>
       <c r="C28">
-        <f>STDEV(C16:C25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>0.10617508443865535</v>
       </c>
       <c r="D28">
-        <f>STDEV(D16:D25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>0.10126514756376533</v>
       </c>
       <c r="E28">
-        <f>STDEV(E16:E25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>7.5000000740740966E-2</v>
       </c>
       <c r="F28">
-        <f>STDEV(F16:F25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>0.16732405431463812</v>
       </c>
       <c r="G28">
-        <f>STDEV(G16:G25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>0.10019271667795357</v>
       </c>
       <c r="H28">
-        <f>STDEV(H16:H25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>9.546022515382932E-2</v>
       </c>
       <c r="I28">
-        <f>STDEV(I16:I25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>8.611111397849483E-2</v>
       </c>
       <c r="J28">
-        <f>STDEV(J16:J25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>0.16374300406847128</v>
       </c>
       <c r="K28">
-        <f>STDEV(K16:K25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>0.10019271667795357</v>
       </c>
       <c r="L28">
-        <f>STDEV(L16:L25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>9.4607703337858451E-2</v>
       </c>
       <c r="M28">
-        <f>STDEV(M16:M25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>6.8098064139197348E-2</v>
       </c>
       <c r="N28">
-        <f>STDEV(N16:N25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>0.17744295420677256</v>
       </c>
       <c r="O28">
-        <f>STDEV(O16:O25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>8.5346067264583991E-2</v>
       </c>
       <c r="P28">
-        <f>STDEV(P16:P25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>0.11317527322315515</v>
       </c>
       <c r="Q28">
-        <f>STDEV(Q16:Q25)/SQRT(10)</f>
+        <f t="shared" si="16"/>
         <v>8.611111397849483E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>0.196448654003127</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>8.611111397849483E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>0.12663679999999999</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>0.21096609999999999</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>0.85714290000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>0.15335840000000001</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>0.85714290000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>0.2202402</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>0.71428570000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>0.34585359999999998</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>0.57142859999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>0.1748159</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>0.21590039999999999</v>
       </c>
@@ -3730,7 +3730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>0.28717819999999999</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>0.1841054</v>
       </c>
@@ -3830,7 +3830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>0.1727737</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>0.85714290000000004</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>63</v>
       </c>
@@ -3889,136 +3889,136 @@
         <v>0.20918286999999997</v>
       </c>
       <c r="C42" s="4">
-        <f t="shared" ref="C42:Q42" si="16">AVERAGE(C32:C41)</f>
+        <f t="shared" ref="C42:Q42" si="17">AVERAGE(C32:C41)</f>
         <v>0.41785714000000002</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.61785714000000014</v>
       </c>
       <c r="E42" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.95714286999999998</v>
       </c>
       <c r="F42" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.27534542000000001</v>
       </c>
       <c r="G42" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.29642856000000001</v>
       </c>
       <c r="H42" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.48749999000000005</v>
       </c>
       <c r="I42" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.88750001000000012</v>
       </c>
       <c r="J42" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.27595955</v>
       </c>
       <c r="K42" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.26785713</v>
       </c>
       <c r="L42" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.50178569999999989</v>
       </c>
       <c r="M42" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.88750001000000012</v>
       </c>
       <c r="N42" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.28539462999999998</v>
       </c>
       <c r="O42" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.30714286000000002</v>
       </c>
       <c r="P42" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.52142856000000004</v>
       </c>
       <c r="Q42" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.87321429999999989</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>62</v>
       </c>
       <c r="B43">
-        <f>STDEV(B32:B41)</f>
+        <f t="shared" ref="B43:Q43" si="18">STDEV(B32:B41)</f>
         <v>6.4977389672357971E-2</v>
       </c>
       <c r="C43">
-        <f>STDEV(C32:C41)</f>
+        <f t="shared" si="18"/>
         <v>0.22338486647807923</v>
       </c>
       <c r="D43">
-        <f>STDEV(D32:D41)</f>
+        <f t="shared" si="18"/>
         <v>0.18136701199101582</v>
       </c>
       <c r="E43">
-        <f>STDEV(E32:E41)</f>
+        <f t="shared" si="18"/>
         <v>6.9006535232268615E-2</v>
       </c>
       <c r="F43">
-        <f>STDEV(F32:F41)</f>
+        <f t="shared" si="18"/>
         <v>6.8560032709651136E-2</v>
       </c>
       <c r="G43">
-        <f>STDEV(G32:G41)</f>
+        <f t="shared" si="18"/>
         <v>0.14290675265588154</v>
       </c>
       <c r="H43">
-        <f>STDEV(H32:H41)</f>
+        <f t="shared" si="18"/>
         <v>0.24772921211277094</v>
       </c>
       <c r="I43">
-        <f>STDEV(I32:I41)</f>
+        <f t="shared" si="18"/>
         <v>0.1472657954792658</v>
       </c>
       <c r="J43">
-        <f>STDEV(J32:J41)</f>
+        <f t="shared" si="18"/>
         <v>6.9459312329421402E-2</v>
       </c>
       <c r="K43">
-        <f>STDEV(K32:K41)</f>
+        <f t="shared" si="18"/>
         <v>0.17107272309547872</v>
       </c>
       <c r="L43">
-        <f>STDEV(L32:L41)</f>
+        <f t="shared" si="18"/>
         <v>0.25705053424219071</v>
       </c>
       <c r="M43">
-        <f>STDEV(M32:M41)</f>
+        <f t="shared" si="18"/>
         <v>0.1472657954792658</v>
       </c>
       <c r="N43">
-        <f>STDEV(N32:N41)</f>
+        <f t="shared" si="18"/>
         <v>8.0022427733063964E-2</v>
       </c>
       <c r="O43">
-        <f>STDEV(O32:O41)</f>
+        <f t="shared" si="18"/>
         <v>0.21309192197473109</v>
       </c>
       <c r="P43">
-        <f>STDEV(P32:P41)</f>
+        <f t="shared" si="18"/>
         <v>0.17833318608932977</v>
       </c>
       <c r="Q43">
-        <f>STDEV(Q32:Q41)</f>
+        <f t="shared" si="18"/>
         <v>0.14197394985574802</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -4027,67 +4027,67 @@
         <v>2.0547654777695316E-2</v>
       </c>
       <c r="C44">
-        <f t="shared" ref="C44:Q44" si="17">C43/SQRT(10)</f>
+        <f t="shared" ref="C44:Q44" si="19">C43/SQRT(10)</f>
         <v>7.0640497288332618E-2</v>
       </c>
       <c r="D44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>5.7353285031067985E-2</v>
       </c>
       <c r="E44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.1821782477062523E-2</v>
       </c>
       <c r="F44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.1680585981814313E-2</v>
       </c>
       <c r="G44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>4.5191083141090237E-2</v>
       </c>
       <c r="H44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>7.8338855323532935E-2</v>
       </c>
       <c r="I44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>4.6569533515100771E-2</v>
       </c>
       <c r="J44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.1964963166998735E-2</v>
       </c>
       <c r="K44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>5.4097945050900348E-2</v>
       </c>
       <c r="L44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>8.128651619684267E-2</v>
       </c>
       <c r="M44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>4.6569533515100771E-2</v>
       </c>
       <c r="N44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.5305313553270672E-2</v>
       </c>
       <c r="O44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>6.738558244230354E-2</v>
       </c>
       <c r="P44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>5.6393905043693786E-2</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>4.4896104995469761E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>2.0547654777695299E-2</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>4.4896104995469761E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>-3.2654827000000002</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>0.45454549999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>1.2795768000000001</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>2.1197480999999998</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>0.81818179999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>1.4929074</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>2.1731619000000002</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>0.54545449999999995</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>0.99888350000000004</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>0.6188053</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>0.50022100000000003</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>0.63636360000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>-38.337144199999997</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>0.44300509999999999</v>
       </c>
@@ -4690,7 +4690,7 @@
         <v>0.90908999999999995</v>
       </c>
     </row>
-    <row r="58" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>63</v>
       </c>
@@ -4699,67 +4699,67 @@
         <v>-3.1976317799999996</v>
       </c>
       <c r="C58" s="4">
-        <f t="shared" ref="C58" si="18">AVERAGE(C48:C57)</f>
+        <f t="shared" ref="C58" si="20">AVERAGE(C48:C57)</f>
         <v>0.23454546999999998</v>
       </c>
       <c r="D58" s="4">
-        <f t="shared" ref="D58" si="19">AVERAGE(D48:D57)</f>
+        <f t="shared" ref="D58" si="21">AVERAGE(D48:D57)</f>
         <v>0.40727273000000003</v>
       </c>
       <c r="E58" s="4">
-        <f t="shared" ref="E58" si="20">AVERAGE(E48:E57)</f>
+        <f t="shared" ref="E58" si="22">AVERAGE(E48:E57)</f>
         <v>0.66636362000000005</v>
       </c>
       <c r="F58" s="4">
-        <f t="shared" ref="F58" si="21">AVERAGE(F48:F57)</f>
+        <f t="shared" ref="F58" si="23">AVERAGE(F48:F57)</f>
         <v>1.8185503899999997</v>
       </c>
       <c r="G58" s="4">
-        <f t="shared" ref="G58" si="22">AVERAGE(G48:G57)</f>
+        <f t="shared" ref="G58" si="24">AVERAGE(G48:G57)</f>
         <v>0.18727274000000002</v>
       </c>
       <c r="H58" s="4">
-        <f t="shared" ref="H58" si="23">AVERAGE(H48:H57)</f>
+        <f t="shared" ref="H58" si="25">AVERAGE(H48:H57)</f>
         <v>0.27272727999999996</v>
       </c>
       <c r="I58" s="4">
-        <f t="shared" ref="I58" si="24">AVERAGE(I48:I57)</f>
+        <f t="shared" ref="I58" si="26">AVERAGE(I48:I57)</f>
         <v>0.61727272</v>
       </c>
       <c r="J58" s="4">
-        <f t="shared" ref="J58" si="25">AVERAGE(J48:J57)</f>
+        <f t="shared" ref="J58" si="27">AVERAGE(J48:J57)</f>
         <v>1.79499656</v>
       </c>
       <c r="K58" s="4">
-        <f t="shared" ref="K58" si="26">AVERAGE(K48:K57)</f>
+        <f t="shared" ref="K58" si="28">AVERAGE(K48:K57)</f>
         <v>0.19727274</v>
       </c>
       <c r="L58" s="4">
-        <f t="shared" ref="L58" si="27">AVERAGE(L48:L57)</f>
+        <f t="shared" ref="L58" si="29">AVERAGE(L48:L57)</f>
         <v>0.28272727999999997</v>
       </c>
       <c r="M58" s="4">
-        <f t="shared" ref="M58" si="28">AVERAGE(M48:M57)</f>
+        <f t="shared" ref="M58" si="30">AVERAGE(M48:M57)</f>
         <v>0.62727272000000001</v>
       </c>
       <c r="N58" s="4">
-        <f t="shared" ref="N58" si="29">AVERAGE(N48:N57)</f>
+        <f t="shared" ref="N58" si="31">AVERAGE(N48:N57)</f>
         <v>1.2085774700000003</v>
       </c>
       <c r="O58" s="4">
-        <f t="shared" ref="O58" si="30">AVERAGE(O48:O57)</f>
+        <f t="shared" ref="O58" si="32">AVERAGE(O48:O57)</f>
         <v>0.26545456000000001</v>
       </c>
       <c r="P58" s="4">
-        <f t="shared" ref="P58" si="31">AVERAGE(P48:P57)</f>
+        <f t="shared" ref="P58" si="33">AVERAGE(P48:P57)</f>
         <v>0.36909092000000004</v>
       </c>
       <c r="Q58" s="4">
-        <f t="shared" ref="Q58" si="32">AVERAGE(Q48:Q57)</f>
+        <f t="shared" ref="Q58" si="34">AVERAGE(Q48:Q57)</f>
         <v>0.64636354000000007</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -4768,67 +4768,67 @@
         <v>12.441242923917827</v>
       </c>
       <c r="C59">
-        <f t="shared" ref="C59:Q59" si="33">STDEV(C48:C57)</f>
+        <f t="shared" ref="C59:Q59" si="35">STDEV(C48:C57)</f>
         <v>0.17859775260108987</v>
       </c>
       <c r="D59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.21254501972633699</v>
       </c>
       <c r="E59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.17158313779445436</v>
       </c>
       <c r="F59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>2.3120633661688181</v>
       </c>
       <c r="G59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>9.2133186183519719E-2</v>
       </c>
       <c r="H59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.12567539702668593</v>
       </c>
       <c r="I59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.12071487653895464</v>
       </c>
       <c r="J59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>2.2566216260591379</v>
       </c>
       <c r="K59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>7.5581625516408901E-2</v>
       </c>
       <c r="L59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.12319960892810236</v>
       </c>
       <c r="M59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.1232405906980034</v>
       </c>
       <c r="N59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.92527465185455648</v>
       </c>
       <c r="O59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.12544137486128465</v>
       </c>
       <c r="P59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.15553455574637345</v>
       </c>
       <c r="Q59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.18168919801664465</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>23</v>
       </c>
@@ -4837,67 +4837,67 @@
         <v>3.9342664563033267</v>
       </c>
       <c r="C60">
-        <f t="shared" ref="C60:Q60" si="34">C59/SQRT(10)</f>
+        <f t="shared" ref="C60:Q60" si="36">C59/SQRT(10)</f>
         <v>5.6477568320670551E-2</v>
       </c>
       <c r="D60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>6.7212636766064288E-2</v>
       </c>
       <c r="E60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>5.425935235089957E-2</v>
       </c>
       <c r="F60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.7311386331729357</v>
       </c>
       <c r="G60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>2.9135071642827838E-2</v>
       </c>
       <c r="H60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>3.9742050045028045E-2</v>
       </c>
       <c r="I60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>3.8173395732912029E-2</v>
       </c>
       <c r="J60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.71360641555396531</v>
       </c>
       <c r="K60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>2.3901008588975221E-2</v>
       </c>
       <c r="L60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>3.8959137105481892E-2</v>
       </c>
       <c r="M60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>3.8972096679025112E-2</v>
       </c>
       <c r="N60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.29259753610797384</v>
       </c>
       <c r="O60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>3.9668045738464774E-2</v>
       </c>
       <c r="P60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>4.9184345102097016E-2</v>
       </c>
       <c r="Q60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>5.7455169198194433E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>0.21797733812069001</v>
       </c>
@@ -4947,17 +4947,17 @@
         <v>5.7455169198194433E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
         <v>58</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>12</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>11</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>17.441532906549071</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
         <v>60</v>
       </c>
@@ -5040,17 +5040,17 @@
         <v>10.273433987114942</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
         <v>58</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
         <v>8</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>1.1425162611450843</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
         <v>13</v>
       </c>
@@ -5090,7 +5090,7 @@
         <v>1.1667447268436897</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
         <v>14</v>
       </c>
@@ -5103,12 +5103,12 @@
         <v>1.6031587558217677</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>37</v>
       </c>
@@ -5119,8 +5119,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B81" s="3"/>
       <c r="C81" s="3" t="s">
         <v>67</v>
@@ -5143,7 +5143,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>38</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>0.36909092000000004</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>39</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>2.4190998031221749E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
         <v>40</v>
       </c>
@@ -5230,7 +5230,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
         <v>41</v>
       </c>
@@ -5253,7 +5253,7 @@
       </c>
       <c r="L85" s="1"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
         <v>42</v>
       </c>
@@ -5276,7 +5276,7 @@
       </c>
       <c r="L86" s="1"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
         <v>43</v>
       </c>
@@ -5299,7 +5299,7 @@
       </c>
       <c r="L87" s="1"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
         <v>44</v>
       </c>
@@ -5322,7 +5322,7 @@
       </c>
       <c r="L88" s="1"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
         <v>45</v>
       </c>
@@ -5345,7 +5345,7 @@
       </c>
       <c r="L89" s="1"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>46</v>
       </c>
@@ -5368,7 +5368,7 @@
       </c>
       <c r="L90" s="1"/>
     </row>
-    <row r="91" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
         <v>47</v>
       </c>
@@ -5391,7 +5391,7 @@
       </c>
       <c r="L91" s="2"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>70</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>74</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>75</v>
       </c>
@@ -5431,11 +5431,11 @@
         <v>2</v>
       </c>
       <c r="D97">
-        <f t="shared" ref="D97:D105" si="35">(C97/10)*0.25</f>
+        <f t="shared" ref="D97:D105" si="37">(C97/10)*0.25</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>76</v>
       </c>
@@ -5450,66 +5450,66 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C99">
         <v>4</v>
       </c>
       <c r="D99">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C100">
         <v>5</v>
       </c>
       <c r="D100">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.125</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C101">
         <v>6</v>
       </c>
       <c r="D101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C102">
         <v>7</v>
       </c>
       <c r="D102">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.17499999999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C103">
         <v>8</v>
       </c>
       <c r="D103">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C104">
         <v>9</v>
       </c>
       <c r="D104">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C105">
         <v>10</v>
       </c>
       <c r="D105">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added previous years' transactin dataset
</commit_message>
<xml_diff>
--- a/data/UseCaseWeighting/7-9/data_points_accuracy_7_11.xlsx
+++ b/data/UseCaseWeighting/7-9/data_points_accuracy_7_11.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17460" windowHeight="8805" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17460" windowHeight="8808" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="False Discovery Rate" sheetId="2" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="data_points_accuracy1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1104,9 +1105,9 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1120,27 +1121,27 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1154,27 +1155,27 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1188,27 +1189,27 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1222,22 +1223,22 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1255,23 +1256,23 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1"/>
-    <col min="20" max="20" width="18.7109375" customWidth="1"/>
-    <col min="25" max="25" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
+    <col min="20" max="20" width="18.6640625" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" customWidth="1"/>
     <col min="26" max="26" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1312,7 +1313,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1350,7 +1351,7 @@
         <v>7.5000000740740966E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1395,7 +1396,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1442,7 +1443,7 @@
         <v>0.883476598</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1489,7 +1490,7 @@
         <v>0.268117713813674</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1536,7 +1537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1581,7 +1582,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1626,7 +1627,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1671,7 +1672,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1716,7 +1717,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1761,7 +1762,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1806,7 +1807,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1851,17 +1852,17 @@
       </c>
       <c r="P13" s="2"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>58</v>
       </c>
@@ -1878,7 +1879,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E18">
         <f>(E4-E2)/SQRT(F4^2/10+F2^2/10)</f>
         <v>2.0897288898007096</v>
@@ -1895,7 +1896,7 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E19">
         <f>(E8-E6)/SQRT(F8^2/10+F6^2/10)</f>
         <v>7.0207075885885919</v>
@@ -1909,7 +1910,7 @@
         <v>17.938296685533214</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E20">
         <f>(E12-E10)/SQRT(F10^2/10+F12^2/10)</f>
         <v>2.5077139058619347</v>
@@ -1923,17 +1924,17 @@
         <v>9.2833765053183352</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
         <v>58</v>
       </c>
@@ -1947,7 +1948,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>12</v>
       </c>
@@ -1960,7 +1961,7 @@
         <v>3.0297345913140425</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>11</v>
       </c>
@@ -1973,7 +1974,7 @@
         <v>3.6129552463040615</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>60</v>
       </c>
@@ -1996,34 +1997,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="X74" sqref="X74"/>
+    <sheetView tabSelected="1" topLeftCell="F24" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" customWidth="1"/>
-    <col min="16" max="16" width="23.85546875" customWidth="1"/>
-    <col min="17" max="17" width="20.28515625" customWidth="1"/>
-    <col min="20" max="20" width="18.7109375" customWidth="1"/>
-    <col min="25" max="25" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" customWidth="1"/>
+    <col min="16" max="16" width="23.88671875" customWidth="1"/>
+    <col min="17" max="17" width="20.33203125" customWidth="1"/>
+    <col min="20" max="20" width="18.6640625" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" customWidth="1"/>
     <col min="26" max="26" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2061,7 +2062,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2099,7 +2100,7 @@
         <v>7.5000000740740966E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2137,7 +2138,7 @@
         <v>8.611111397849483E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2175,7 +2176,7 @@
         <v>6.8098064139197348E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>8.611111397849483E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2251,7 +2252,7 @@
         <v>2.1821782477062523E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2289,7 +2290,7 @@
         <v>4.6569533515100771E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2327,7 +2328,7 @@
         <v>4.6569533515100771E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2365,7 +2366,7 @@
         <v>4.4896104995469761E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2403,7 +2404,7 @@
         <v>5.425935235089957E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2441,7 +2442,7 @@
         <v>3.8173395732912029E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2479,7 +2480,7 @@
         <v>3.8972096679025112E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2517,7 +2518,7 @@
         <v>5.7455169198194433E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2570,7 +2571,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>0.27706659</v>
       </c>
@@ -2620,7 +2621,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>0.73431679999999999</v>
       </c>
@@ -2670,7 +2671,7 @@
         <v>0.66666669999999995</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>5.3700350000000001E-2</v>
       </c>
@@ -2720,7 +2721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>1.01997396</v>
       </c>
@@ -2770,7 +2771,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>1.8482500399999999</v>
       </c>
@@ -2820,7 +2821,7 @@
         <v>0.3333333</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>0.82374561999999996</v>
       </c>
@@ -2870,7 +2871,7 @@
         <v>0.3333333</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>0.27362692</v>
       </c>
@@ -2920,7 +2921,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>3.9690900000000001E-2</v>
       </c>
@@ -2970,7 +2971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>1.5832008500000001</v>
       </c>
@@ -3020,7 +3021,7 @@
         <v>0.66666669999999995</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>0.49117488999999998</v>
       </c>
@@ -3070,76 +3071,76 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B26" s="4">
-        <f>AVERAGE(B16:B25)</f>
+        <f t="shared" ref="B26:Q26" si="0">AVERAGE(B16:B25)</f>
         <v>0.71447469200000002</v>
       </c>
       <c r="C26" s="4">
-        <f t="shared" ref="C26" si="0">AVERAGE(C16:C25)</f>
+        <f t="shared" si="0"/>
         <v>0.44166665999999999</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" ref="D26" si="1">AVERAGE(D16:D25)</f>
+        <f t="shared" si="0"/>
         <v>0.49166665999999992</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" ref="E26" si="2">AVERAGE(E16:E25)</f>
+        <f t="shared" si="0"/>
         <v>0.75833334000000008</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" ref="F26" si="3">AVERAGE(F16:F25)</f>
+        <f t="shared" si="0"/>
         <v>0.88240377000000014</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" ref="G26" si="4">AVERAGE(G16:G25)</f>
+        <f t="shared" si="0"/>
         <v>0.30833333000000002</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" ref="H26" si="5">AVERAGE(H16:H25)</f>
+        <f t="shared" si="0"/>
         <v>0.35833333000000001</v>
       </c>
       <c r="I26" s="4">
-        <f t="shared" ref="I26" si="6">AVERAGE(I16:I25)</f>
+        <f t="shared" si="0"/>
         <v>0.47499999999999998</v>
       </c>
       <c r="J26" s="4">
-        <f t="shared" ref="J26" si="7">AVERAGE(J16:J25)</f>
+        <f t="shared" si="0"/>
         <v>0.883476598</v>
       </c>
       <c r="K26" s="4">
-        <f t="shared" ref="K26" si="8">AVERAGE(K16:K25)</f>
+        <f t="shared" si="0"/>
         <v>0.30833333000000002</v>
       </c>
       <c r="L26" s="4">
-        <f t="shared" ref="L26" si="9">AVERAGE(L16:L25)</f>
+        <f t="shared" si="0"/>
         <v>0.33333332999999998</v>
       </c>
       <c r="M26" s="4">
-        <f t="shared" ref="M26" si="10">AVERAGE(M16:M25)</f>
+        <f t="shared" si="0"/>
         <v>0.55833332999999996</v>
       </c>
       <c r="N26" s="4">
-        <f t="shared" ref="N26" si="11">AVERAGE(N16:N25)</f>
+        <f t="shared" si="0"/>
         <v>0.89263809100000002</v>
       </c>
       <c r="O26" s="4">
-        <f t="shared" ref="O26" si="12">AVERAGE(O16:O25)</f>
+        <f t="shared" si="0"/>
         <v>0.21666667000000001</v>
       </c>
       <c r="P26" s="4">
-        <f t="shared" ref="P26" si="13">AVERAGE(P16:P25)</f>
+        <f t="shared" si="0"/>
         <v>0.33333333999999998</v>
       </c>
       <c r="Q26" s="4">
-        <f t="shared" ref="Q26" si="14">AVERAGE(Q16:Q25)</f>
+        <f t="shared" si="0"/>
         <v>0.47499999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -3148,136 +3149,136 @@
         <v>0.62122518992423703</v>
       </c>
       <c r="C27">
-        <f t="shared" ref="C27:Q27" si="15">STDEV(C16:C25)</f>
+        <f t="shared" ref="C27:Q27" si="1">STDEV(C16:C25)</f>
         <v>0.33575509758685118</v>
       </c>
       <c r="D27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="1"/>
         <v>0.32022851389454948</v>
       </c>
       <c r="E27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="1"/>
         <v>0.23717082685505708</v>
       </c>
       <c r="F27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="1"/>
         <v>0.52912511896798065</v>
       </c>
       <c r="G27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="1"/>
         <v>0.31683718966227237</v>
       </c>
       <c r="H27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="1"/>
         <v>0.30187173743859808</v>
       </c>
       <c r="I27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="1"/>
         <v>0.27230725202640726</v>
       </c>
       <c r="J27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="1"/>
         <v>0.51780084377458679</v>
       </c>
       <c r="K27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="1"/>
         <v>0.31683718966227237</v>
       </c>
       <c r="L27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="1"/>
         <v>0.2991758267451472</v>
       </c>
       <c r="M27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="1"/>
         <v>0.21534498692809723</v>
       </c>
       <c r="N27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="1"/>
         <v>0.56112389004235763</v>
       </c>
       <c r="O27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="1"/>
         <v>0.26988796189402181</v>
       </c>
       <c r="P27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="1"/>
         <v>0.35789163819703612</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="1"/>
         <v>0.27230725202640726</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>23</v>
       </c>
       <c r="B28">
-        <f t="shared" ref="B28:Q28" si="16">STDEV(B16:B25)/SQRT(10)</f>
+        <f t="shared" ref="B28:Q28" si="2">STDEV(B16:B25)/SQRT(10)</f>
         <v>0.19644865400312733</v>
       </c>
       <c r="C28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>0.10617508443865535</v>
       </c>
       <c r="D28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>0.10126514756376533</v>
       </c>
       <c r="E28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>7.5000000740740966E-2</v>
       </c>
       <c r="F28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>0.16732405431463812</v>
       </c>
       <c r="G28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>0.10019271667795357</v>
       </c>
       <c r="H28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>9.546022515382932E-2</v>
       </c>
       <c r="I28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>8.611111397849483E-2</v>
       </c>
       <c r="J28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>0.16374300406847128</v>
       </c>
       <c r="K28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>0.10019271667795357</v>
       </c>
       <c r="L28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>9.4607703337858451E-2</v>
       </c>
       <c r="M28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>6.8098064139197348E-2</v>
       </c>
       <c r="N28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>0.17744295420677256</v>
       </c>
       <c r="O28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>8.5346067264583991E-2</v>
       </c>
       <c r="P28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>0.11317527322315515</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>8.611111397849483E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>0.196448654003127</v>
       </c>
@@ -3327,7 +3328,7 @@
         <v>8.611111397849483E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -3380,7 +3381,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>0.12663679999999999</v>
       </c>
@@ -3430,7 +3431,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>0.21096609999999999</v>
       </c>
@@ -3480,7 +3481,7 @@
         <v>0.85714290000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>0.15335840000000001</v>
       </c>
@@ -3530,7 +3531,7 @@
         <v>0.85714290000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>0.2202402</v>
       </c>
@@ -3580,7 +3581,7 @@
         <v>0.71428570000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>0.34585359999999998</v>
       </c>
@@ -3630,7 +3631,7 @@
         <v>0.57142859999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>0.1748159</v>
       </c>
@@ -3680,7 +3681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>0.21590039999999999</v>
       </c>
@@ -3730,7 +3731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>0.28717819999999999</v>
       </c>
@@ -3780,7 +3781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>0.1841054</v>
       </c>
@@ -3830,7 +3831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>0.1727737</v>
       </c>
@@ -3880,7 +3881,7 @@
         <v>0.85714290000000004</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>63</v>
       </c>
@@ -3889,136 +3890,136 @@
         <v>0.20918286999999997</v>
       </c>
       <c r="C42" s="4">
-        <f t="shared" ref="C42:Q42" si="17">AVERAGE(C32:C41)</f>
+        <f t="shared" ref="C42:Q42" si="3">AVERAGE(C32:C41)</f>
         <v>0.41785714000000002</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="3"/>
         <v>0.61785714000000014</v>
       </c>
       <c r="E42" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="3"/>
         <v>0.95714286999999998</v>
       </c>
       <c r="F42" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="3"/>
         <v>0.27534542000000001</v>
       </c>
       <c r="G42" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="3"/>
         <v>0.29642856000000001</v>
       </c>
       <c r="H42" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="3"/>
         <v>0.48749999000000005</v>
       </c>
       <c r="I42" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="3"/>
         <v>0.88750001000000012</v>
       </c>
       <c r="J42" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="3"/>
         <v>0.27595955</v>
       </c>
       <c r="K42" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="3"/>
         <v>0.26785713</v>
       </c>
       <c r="L42" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="3"/>
         <v>0.50178569999999989</v>
       </c>
       <c r="M42" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="3"/>
         <v>0.88750001000000012</v>
       </c>
       <c r="N42" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="3"/>
         <v>0.28539462999999998</v>
       </c>
       <c r="O42" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="3"/>
         <v>0.30714286000000002</v>
       </c>
       <c r="P42" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="3"/>
         <v>0.52142856000000004</v>
       </c>
       <c r="Q42" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="3"/>
         <v>0.87321429999999989</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>62</v>
       </c>
       <c r="B43">
-        <f t="shared" ref="B43:Q43" si="18">STDEV(B32:B41)</f>
+        <f>STDEV(B32:B41)</f>
         <v>6.4977389672357971E-2</v>
       </c>
       <c r="C43">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="C43:Q43" si="4">STDEV(C32:C41)</f>
         <v>0.22338486647807923</v>
       </c>
       <c r="D43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="4"/>
         <v>0.18136701199101582</v>
       </c>
       <c r="E43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="4"/>
         <v>6.9006535232268615E-2</v>
       </c>
       <c r="F43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="4"/>
         <v>6.8560032709651136E-2</v>
       </c>
       <c r="G43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="4"/>
         <v>0.14290675265588154</v>
       </c>
       <c r="H43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="4"/>
         <v>0.24772921211277094</v>
       </c>
       <c r="I43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="4"/>
         <v>0.1472657954792658</v>
       </c>
       <c r="J43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="4"/>
         <v>6.9459312329421402E-2</v>
       </c>
       <c r="K43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="4"/>
         <v>0.17107272309547872</v>
       </c>
       <c r="L43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="4"/>
         <v>0.25705053424219071</v>
       </c>
       <c r="M43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="4"/>
         <v>0.1472657954792658</v>
       </c>
       <c r="N43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="4"/>
         <v>8.0022427733063964E-2</v>
       </c>
       <c r="O43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="4"/>
         <v>0.21309192197473109</v>
       </c>
       <c r="P43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="4"/>
         <v>0.17833318608932977</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="4"/>
         <v>0.14197394985574802</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -4027,67 +4028,67 @@
         <v>2.0547654777695316E-2</v>
       </c>
       <c r="C44">
-        <f t="shared" ref="C44:Q44" si="19">C43/SQRT(10)</f>
+        <f t="shared" ref="C44:Q44" si="5">C43/SQRT(10)</f>
         <v>7.0640497288332618E-2</v>
       </c>
       <c r="D44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="5"/>
         <v>5.7353285031067985E-2</v>
       </c>
       <c r="E44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="5"/>
         <v>2.1821782477062523E-2</v>
       </c>
       <c r="F44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="5"/>
         <v>2.1680585981814313E-2</v>
       </c>
       <c r="G44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="5"/>
         <v>4.5191083141090237E-2</v>
       </c>
       <c r="H44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="5"/>
         <v>7.8338855323532935E-2</v>
       </c>
       <c r="I44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="5"/>
         <v>4.6569533515100771E-2</v>
       </c>
       <c r="J44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="5"/>
         <v>2.1964963166998735E-2</v>
       </c>
       <c r="K44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="5"/>
         <v>5.4097945050900348E-2</v>
       </c>
       <c r="L44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="5"/>
         <v>8.128651619684267E-2</v>
       </c>
       <c r="M44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="5"/>
         <v>4.6569533515100771E-2</v>
       </c>
       <c r="N44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="5"/>
         <v>2.5305313553270672E-2</v>
       </c>
       <c r="O44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="5"/>
         <v>6.738558244230354E-2</v>
       </c>
       <c r="P44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="5"/>
         <v>5.6393905043693786E-2</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="19"/>
+        <f t="shared" si="5"/>
         <v>4.4896104995469761E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B45">
         <v>2.0547654777695299E-2</v>
       </c>
@@ -4137,7 +4138,7 @@
         <v>4.4896104995469761E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -4190,7 +4191,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>-3.2654827000000002</v>
       </c>
@@ -4240,7 +4241,7 @@
         <v>0.45454549999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>1.2795768000000001</v>
       </c>
@@ -4290,7 +4291,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>2.1197480999999998</v>
       </c>
@@ -4340,7 +4341,7 @@
         <v>0.81818179999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>1.4929074</v>
       </c>
@@ -4390,7 +4391,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B52">
         <v>2.1731619000000002</v>
       </c>
@@ -4440,7 +4441,7 @@
         <v>0.54545449999999995</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B53">
         <v>0.99888350000000004</v>
       </c>
@@ -4490,7 +4491,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>0.6188053</v>
       </c>
@@ -4540,7 +4541,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>0.50022100000000003</v>
       </c>
@@ -4590,7 +4591,7 @@
         <v>0.63636360000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B56">
         <v>-38.337144199999997</v>
       </c>
@@ -4640,7 +4641,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B57">
         <v>0.44300509999999999</v>
       </c>
@@ -4690,76 +4691,76 @@
         <v>0.90908999999999995</v>
       </c>
     </row>
-    <row r="58" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B58" s="4">
-        <f>AVERAGE(B48:B57)</f>
+        <f t="shared" ref="B58:Q58" si="6">AVERAGE(B48:B57)</f>
         <v>-3.1976317799999996</v>
       </c>
       <c r="C58" s="4">
-        <f t="shared" ref="C58" si="20">AVERAGE(C48:C57)</f>
+        <f t="shared" si="6"/>
         <v>0.23454546999999998</v>
       </c>
       <c r="D58" s="4">
-        <f t="shared" ref="D58" si="21">AVERAGE(D48:D57)</f>
+        <f t="shared" si="6"/>
         <v>0.40727273000000003</v>
       </c>
       <c r="E58" s="4">
-        <f t="shared" ref="E58" si="22">AVERAGE(E48:E57)</f>
+        <f t="shared" si="6"/>
         <v>0.66636362000000005</v>
       </c>
       <c r="F58" s="4">
-        <f t="shared" ref="F58" si="23">AVERAGE(F48:F57)</f>
+        <f t="shared" si="6"/>
         <v>1.8185503899999997</v>
       </c>
       <c r="G58" s="4">
-        <f t="shared" ref="G58" si="24">AVERAGE(G48:G57)</f>
+        <f t="shared" si="6"/>
         <v>0.18727274000000002</v>
       </c>
       <c r="H58" s="4">
-        <f t="shared" ref="H58" si="25">AVERAGE(H48:H57)</f>
+        <f t="shared" si="6"/>
         <v>0.27272727999999996</v>
       </c>
       <c r="I58" s="4">
-        <f t="shared" ref="I58" si="26">AVERAGE(I48:I57)</f>
+        <f t="shared" si="6"/>
         <v>0.61727272</v>
       </c>
       <c r="J58" s="4">
-        <f t="shared" ref="J58" si="27">AVERAGE(J48:J57)</f>
+        <f t="shared" si="6"/>
         <v>1.79499656</v>
       </c>
       <c r="K58" s="4">
-        <f t="shared" ref="K58" si="28">AVERAGE(K48:K57)</f>
+        <f t="shared" si="6"/>
         <v>0.19727274</v>
       </c>
       <c r="L58" s="4">
-        <f t="shared" ref="L58" si="29">AVERAGE(L48:L57)</f>
+        <f t="shared" si="6"/>
         <v>0.28272727999999997</v>
       </c>
       <c r="M58" s="4">
-        <f t="shared" ref="M58" si="30">AVERAGE(M48:M57)</f>
+        <f t="shared" si="6"/>
         <v>0.62727272000000001</v>
       </c>
       <c r="N58" s="4">
-        <f t="shared" ref="N58" si="31">AVERAGE(N48:N57)</f>
+        <f t="shared" si="6"/>
         <v>1.2085774700000003</v>
       </c>
       <c r="O58" s="4">
-        <f t="shared" ref="O58" si="32">AVERAGE(O48:O57)</f>
+        <f t="shared" si="6"/>
         <v>0.26545456000000001</v>
       </c>
       <c r="P58" s="4">
-        <f t="shared" ref="P58" si="33">AVERAGE(P48:P57)</f>
+        <f t="shared" si="6"/>
         <v>0.36909092000000004</v>
       </c>
       <c r="Q58" s="4">
-        <f t="shared" ref="Q58" si="34">AVERAGE(Q48:Q57)</f>
+        <f t="shared" si="6"/>
         <v>0.64636354000000007</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -4768,67 +4769,67 @@
         <v>12.441242923917827</v>
       </c>
       <c r="C59">
-        <f t="shared" ref="C59:Q59" si="35">STDEV(C48:C57)</f>
+        <f t="shared" ref="C59:Q59" si="7">STDEV(C48:C57)</f>
         <v>0.17859775260108987</v>
       </c>
       <c r="D59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>0.21254501972633699</v>
       </c>
       <c r="E59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>0.17158313779445436</v>
       </c>
       <c r="F59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>2.3120633661688181</v>
       </c>
       <c r="G59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>9.2133186183519719E-2</v>
       </c>
       <c r="H59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>0.12567539702668593</v>
       </c>
       <c r="I59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>0.12071487653895464</v>
       </c>
       <c r="J59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>2.2566216260591379</v>
       </c>
       <c r="K59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>7.5581625516408901E-2</v>
       </c>
       <c r="L59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>0.12319960892810236</v>
       </c>
       <c r="M59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>0.1232405906980034</v>
       </c>
       <c r="N59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>0.92527465185455648</v>
       </c>
       <c r="O59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>0.12544137486128465</v>
       </c>
       <c r="P59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>0.15553455574637345</v>
       </c>
       <c r="Q59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>0.18168919801664465</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>23</v>
       </c>
@@ -4837,67 +4838,67 @@
         <v>3.9342664563033267</v>
       </c>
       <c r="C60">
-        <f t="shared" ref="C60:Q60" si="36">C59/SQRT(10)</f>
+        <f t="shared" ref="C60:Q60" si="8">C59/SQRT(10)</f>
         <v>5.6477568320670551E-2</v>
       </c>
       <c r="D60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>6.7212636766064288E-2</v>
       </c>
       <c r="E60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>5.425935235089957E-2</v>
       </c>
       <c r="F60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>0.7311386331729357</v>
       </c>
       <c r="G60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>2.9135071642827838E-2</v>
       </c>
       <c r="H60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>3.9742050045028045E-2</v>
       </c>
       <c r="I60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>3.8173395732912029E-2</v>
       </c>
       <c r="J60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>0.71360641555396531</v>
       </c>
       <c r="K60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>2.3901008588975221E-2</v>
       </c>
       <c r="L60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>3.8959137105481892E-2</v>
       </c>
       <c r="M60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>3.8972096679025112E-2</v>
       </c>
       <c r="N60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>0.29259753610797384</v>
       </c>
       <c r="O60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>3.9668045738464774E-2</v>
       </c>
       <c r="P60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>4.9184345102097016E-2</v>
       </c>
       <c r="Q60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>5.7455169198194433E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B61">
         <v>0.21797733812069001</v>
       </c>
@@ -4947,17 +4948,17 @@
         <v>5.7455169198194433E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E64" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E65" t="s">
         <v>58</v>
       </c>
@@ -4980,7 +4981,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D66" t="s">
         <v>12</v>
       </c>
@@ -5006,7 +5007,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
         <v>11</v>
       </c>
@@ -5023,7 +5024,7 @@
         <v>17.441532906549071</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
         <v>60</v>
       </c>
@@ -5040,17 +5041,17 @@
         <v>10.273433987114942</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E72" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E73" t="s">
         <v>58</v>
       </c>
@@ -5064,7 +5065,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
         <v>8</v>
       </c>
@@ -5077,7 +5078,7 @@
         <v>1.1425162611450843</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
         <v>13</v>
       </c>
@@ -5090,7 +5091,7 @@
         <v>1.1667447268436897</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D76" t="s">
         <v>14</v>
       </c>
@@ -5103,12 +5104,12 @@
         <v>1.6031587558217677</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>37</v>
       </c>
@@ -5119,8 +5120,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B81" s="3"/>
       <c r="C81" s="3" t="s">
         <v>67</v>
@@ -5143,7 +5144,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B82" s="1" t="s">
         <v>38</v>
       </c>
@@ -5172,7 +5173,7 @@
         <v>0.36909092000000004</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B83" s="1" t="s">
         <v>39</v>
       </c>
@@ -5201,7 +5202,7 @@
         <v>2.4190998031221749E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B84" s="1" t="s">
         <v>40</v>
       </c>
@@ -5230,7 +5231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B85" s="1" t="s">
         <v>41</v>
       </c>
@@ -5253,7 +5254,7 @@
       </c>
       <c r="L85" s="1"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B86" s="1" t="s">
         <v>42</v>
       </c>
@@ -5276,7 +5277,7 @@
       </c>
       <c r="L86" s="1"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B87" s="1" t="s">
         <v>43</v>
       </c>
@@ -5299,7 +5300,7 @@
       </c>
       <c r="L87" s="1"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
         <v>44</v>
       </c>
@@ -5322,7 +5323,7 @@
       </c>
       <c r="L88" s="1"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B89" s="1" t="s">
         <v>45</v>
       </c>
@@ -5345,7 +5346,7 @@
       </c>
       <c r="L89" s="1"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B90" s="1" t="s">
         <v>46</v>
       </c>
@@ -5368,7 +5369,7 @@
       </c>
       <c r="L90" s="1"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B91" s="2" t="s">
         <v>47</v>
       </c>
@@ -5391,7 +5392,7 @@
       </c>
       <c r="L91" s="2"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>70</v>
       </c>
@@ -5405,7 +5406,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>74</v>
       </c>
@@ -5420,7 +5421,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>75</v>
       </c>
@@ -5431,11 +5432,11 @@
         <v>2</v>
       </c>
       <c r="D97">
-        <f t="shared" ref="D97:D105" si="37">(C97/10)*0.25</f>
+        <f t="shared" ref="D97:D105" si="9">(C97/10)*0.25</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>76</v>
       </c>
@@ -5450,66 +5451,66 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C99">
         <v>4</v>
       </c>
       <c r="D99">
-        <f t="shared" si="37"/>
+        <f t="shared" si="9"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C100">
         <v>5</v>
       </c>
       <c r="D100">
-        <f t="shared" si="37"/>
+        <f t="shared" si="9"/>
         <v>0.125</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C101">
         <v>6</v>
       </c>
       <c r="D101">
-        <f t="shared" si="37"/>
+        <f t="shared" si="9"/>
         <v>0.15</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C102">
         <v>7</v>
       </c>
       <c r="D102">
-        <f t="shared" si="37"/>
+        <f t="shared" si="9"/>
         <v>0.17499999999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C103">
         <v>8</v>
       </c>
       <c r="D103">
-        <f t="shared" si="37"/>
+        <f t="shared" si="9"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C104">
         <v>9</v>
       </c>
       <c r="D104">
-        <f t="shared" si="37"/>
+        <f t="shared" si="9"/>
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C105">
         <v>10</v>
       </c>
       <c r="D105">
-        <f t="shared" si="37"/>
+        <f t="shared" si="9"/>
         <v>0.25</v>
       </c>
     </row>

</xml_diff>